<commit_message>
Docs de excel ejecutar desde(3908)
</commit_message>
<xml_diff>
--- a/AVT_TRAKING-b5a19f52c2a889d8592336db032ecf143043f8f5/AVT_TRAKING/AVT_TRAKING/Documents/ExcelDoc/InvoicePieces.xlsx
+++ b/AVT_TRAKING-b5a19f52c2a889d8592336db032ecf143043f8f5/AVT_TRAKING/AVT_TRAKING/Documents/ExcelDoc/InvoicePieces.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\source\repos\AVT_TRAKING2\AVT_TRAKING-b5a19f52c2a889d8592336db032ecf143043f8f5\AVT_TRAKING\AVT_TRAKING\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\source\repos\AVT_TRAKING\AVT_TRAKING-b5a19f52c2a889d8592336db032ecf143043f8f5\AVT_TRAKING\AVT_TRAKING\Documents\ExcelDoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE776276-DA66-468F-BF09-16D2136E4355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E74F4DF-7776-4ACC-8DE0-90468BA4B7B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{38B5D577-474C-4399-9CA6-7E2D0DD88AA4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" activeTab="1" xr2:uid="{38B5D577-474C-4399-9CA6-7E2D0DD88AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Pieces" sheetId="3" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>Type (O,M,T,C)</t>
   </si>
@@ -78,33 +78,6 @@
     <t>Work</t>
   </si>
   <si>
-    <t>3349518</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>P1TICL Chlorination</t>
-  </si>
-  <si>
-    <t>Mod</t>
-  </si>
-  <si>
-    <t>1141</t>
-  </si>
-  <si>
-    <t>01/04/2022</t>
-  </si>
-  <si>
-    <t>Build</t>
-  </si>
-  <si>
-    <t>1140</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>Tag #</t>
   </si>
   <si>
@@ -133,15 +106,6 @@
   </si>
   <si>
     <t>Labor WO / Network #</t>
-  </si>
-  <si>
-    <t>01/03/2022</t>
-  </si>
-  <si>
-    <t>1139</t>
-  </si>
-  <si>
-    <t>03/01/2022</t>
   </si>
   <si>
     <t>SRLs</t>
@@ -520,7 +484,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -818,30 +782,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15DBB563-4785-449F-AAF5-1BCA63F1C3B4}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -852,21 +816,17 @@
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="18">
-        <v>44569</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="K1" s="18"/>
       <c r="L1" s="7"/>
       <c r="M1" s="23"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="21">
-        <v>44569</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="K2" s="21"/>
       <c r="L2" s="22">
         <f>K2-(K1-1)</f>
         <v>1</v>
@@ -894,7 +854,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
@@ -907,7 +867,7 @@
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" s="27" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="M4" s="27"/>
       <c r="N4" s="27"/>
@@ -920,16 +880,16 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>2</v>
@@ -938,13 +898,13 @@
         <v>3</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>5</v>
@@ -953,83 +913,7 @@
         <v>6</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6">
-        <v>0.09</v>
-      </c>
-      <c r="J6">
-        <v>57</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="J7">
-        <v>233</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7" t="s">
-        <v>13</v>
-      </c>
-      <c r="M7" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -1108,19 +992,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F57257B-8A29-41E9-A359-4D17BE936CD4}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.140625" customWidth="1"/>
@@ -1128,7 +1012,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -1138,11 +1022,9 @@
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="10">
-        <v>44569</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J1" s="10"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
@@ -1154,11 +1036,9 @@
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
       <c r="I2" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="13">
-        <v>44569</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="J2" s="13"/>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1175,7 +1055,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
@@ -1185,19 +1065,19 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>2</v>
@@ -1206,61 +1086,9 @@
         <v>3</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="I5" s="17"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" t="s">
-        <v>15</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>